<commit_message>
Actualización flujo de trabajo
</commit_message>
<xml_diff>
--- a/BrailleTech_Documentacion/Documentacion - Construccion/Flujo de trabajo - BrailleTech.xlsx
+++ b/BrailleTech_Documentacion/Documentacion - Construccion/Flujo de trabajo - BrailleTech.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6ad90d8d74be4ced/Documentos/Proyectos Github 6to/BrailleTech/BrailleTech_Documentacion/Documentacion - Construccion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eddya\source\repos\BrailleTech\BrailleTech_Documentacion\Documentacion - Construccion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="108" documentId="8_{10BD72DA-26FE-4F91-9634-C76F7E360ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CC7B13C-A7C3-4EE0-AB59-7A147DADF3C4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426BECD0-9ED9-4440-9F57-2C34C27E1FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2A4DEB56-B447-4768-8E44-E3C730C22452}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="62">
   <si>
     <t>WORK-FLOW</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Implementación</t>
   </si>
   <si>
-    <t>Iteración 1</t>
-  </si>
-  <si>
     <t>Max Carrion - Analista</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
   </si>
   <si>
     <t>Milton Pástor, Fredviner Bailon - Testers</t>
-  </si>
-  <si>
-    <t>Historia de usuario 1, 2, 3 y 4</t>
   </si>
   <si>
     <t>Configuración de entorno de desarrollo
@@ -144,28 +138,167 @@
     <t>ESTIMACIÓN</t>
   </si>
   <si>
+    <t>ISWD633 CONTRUCCIÓN Y EVOLUCÍON DEL SOFTWARE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRADUCTOR VERSIÓN: 1.0 </t>
+  </si>
+  <si>
+    <t>FECHA DE PUBLICACIÓN:</t>
+  </si>
+  <si>
+    <t>AUTOR:</t>
+  </si>
+  <si>
+    <t>TEMA:</t>
+  </si>
+  <si>
+    <t>FLUJO DE TRABAJO</t>
+  </si>
+  <si>
+    <t>BrailleTech</t>
+  </si>
+  <si>
+    <t>ESTADO</t>
+  </si>
+  <si>
+    <t>COMPLETADO</t>
+  </si>
+  <si>
+    <t>Historia de usuario 1, 2 y 4</t>
+  </si>
+  <si>
+    <t>Historia de usuario 3, 5 y 6</t>
+  </si>
+  <si>
+    <t>3 horas (1 hora por HU)</t>
+  </si>
+  <si>
+    <t>6 horas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Dividir el proyecto en directorios como src, tests, config, etc.
+2. Crear módulos específicos para funcionalidades como conversión de texto (braille.js, 
+brailleMap.js), manejo de la interfaz (index.js), y estilos (style.css). 
+3. Implementar patrones de diseño como MVC (Modelo-Vista-Controlador) o similar 
+para separar las responsabilidades.
+4. Documentar la estructura del proyecto para facilitar la comprensión y colaboración. 
+5. Diseñar el algoritmo de conversión.
+</t>
+  </si>
+  <si>
+    <t>1. Codificar la función toBraille en braille.js y asegurarse de que 
+maneje correctamente todos los caracteres especificados. 
+2. Incluir validaciones en eventHandlers.js para verificar que el texto 
+en español contiene solo caracteres válidos antes de la conversión. 
+3. Conectar la funcionalidad de conversión con la interfaz gráfica 
+(index.html y eventHandlers.js), incluyendo la gestión de eventos del botón "Traducir".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Codigo fuente de los modulos braille.js (Funcion toBraille y funciones auxiliares)
+Modulo brailleMap para realizar el mapeo.
+Modulo translate que implenta los metodos del braille.js
+</t>
+  </si>
+  <si>
+    <t>Modulo utils.js con funciones utilitarias, como la generación de señalética y la creación de elementos en espejo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Casos de prueba: 
+CP001, CP002, CP03, CP008, CP009, 
+CP010, CP011, CP012, CP013, CP018 
+Pruebas unitarias de 
+braille.test.js: 
+PU001, PU002, PU003, PU004, PU005, PU006, PU007, PU008, PU009, PU010, PU011, PU012, PU013, PU014, PU015, 
+PU016, PU017, PU018, PU019, PU020, PU021, PU022 </t>
+  </si>
+  <si>
+    <t>15 horas</t>
+  </si>
+  <si>
+    <t>8 horas</t>
+  </si>
+  <si>
+    <t>Historia de usuario 7 y 8</t>
+  </si>
+  <si>
+    <t>1. Identificar y documentar las necesidades y requerimientos del usuario en esta iteración se determino que es necesario la generación de señaletica Braille y generación de señaletica con espejo.
+2. Elaborar las historias de usuario con criterios de aceptación claros.
+3. Realizar reuniones de revisión con el equipo de desarrollo para asegurar el entendimiento de las historias de usuario.
+4. Revisar y ajustar las historias de usuario basándose en la retroalimentación del equipo.
+5. Aprobar las historias de usuario finales para su implementación.</t>
+  </si>
+  <si>
+    <t>2 horas</t>
+  </si>
+  <si>
+    <t>Estructura del proyecto por Capas o modulos</t>
+  </si>
+  <si>
+    <t>Arquitectura del sistema
+Dependencias adicinales: html2canvas y jsPDF
+Flujo de Datos
+Definición de patrones de diseño</t>
+  </si>
+  <si>
+    <t>1. Diseño de una arquitectura por capas, en la que cada capa tiene responsabilidades específicas.
+2. Análisis de herramientas utilizadas para generar imágenes y PDFs a partir de elementos HTML.
+3. Creación del flujo de datos.
+4. Definición del encapsulamiento y la separación de responsabilidades.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Codificar la función createSignageElement en utils.js para generar 
+el elemento HTML correspondiente.
+2. Utilizar html2canvas para convertir el elemento HTML a imagen y 
+permitir su descarga. 
+3. Incluir validaciones en eventHandlers.js para asegurar que el texto 
+en español contiene solo caracteres válidos antes de la generación de señalética. 
+4. Conectar la funcionalidad de generación de señalética con la 
+interfaz gráfica (index.html y eventHandlers.js), incluyendo la gestión de eventos del botón "Descargar Señalética". 
+5. Codificar la función createMirrorElement en utils.js para generar el 
+elemento HTML correspondiente.
+6.  Utilizar jsPDF para convertir el elemento HTML a PDF y permitir 
+su descarga. 
+7.  Incluir validaciones en eventHandlers.js para asegurar que el texto 
+en español contiene solo caracteres válidos antes de la generación de impresión en espejo.
+8. Conectar la funcionalidad de generación de impresión en espejo 
+con la interfaz gráfica (index.html y eventHandlers.js), incluyendo la gestión de eventos del botón "Descargar Formato Espejo". </t>
+  </si>
+  <si>
+    <t>Casos de prueba: 
+CP004, CP005, CP006 y CP007</t>
+  </si>
+  <si>
+    <t>1. Verificar la correcta codificación de la función createSignageElement en utils.js para asegurar que genera el elemento HTML adecuado.
+2. Probar la utilización de html2canvas para convertir el elemento HTML en una imagen y validar la funcionalidad de descarga.
+3. Revisar las validaciones en eventHandlers.js para confirmar que el texto en español contiene solo caracteres válidos antes de la generación de señalética.
+4. Validar la conexión de la funcionalidad de generación de señalética con la interfaz gráfica (index.html y eventHandlers.js), incluyendo la gestión de eventos del botón "Descargar Señalética".
+5. Comprobar la correcta codificación de la función createMirrorElement en utils.js para asegurar que genera el elemento HTML adecuado.
+6. Probar la utilización de jsPDF para convertir el elemento HTML en un PDF y validar la funcionalidad de descarga.
+7. Revisar las validaciones en eventHandlers.js para confirmar que el texto en español contiene solo caracteres válidos antes de la generación de impresión en espejo.
+8. Validar la conexión de la funcionalidad de generación de impresión en espejo con la interfaz gráfica (index.html y eventHandlers.js), incluyendo la gestión de eventos del botón "Descargar Formato Espejo".</t>
+  </si>
+  <si>
+    <t>1. Verificar la correcta codificación de la función toBraille en braille.js, asegurándose de que maneje correctamente todos los caracteres especificados.
+2. Revisar las validaciones en eventHandlers.js para confirmar que el texto en español contiene solo caracteres válidos antes de la conversión.
+3. Validar la conexión de la funcionalidad de conversión a braille con la interfaz gráfica (index.html y eventHandlers.js), incluyendo la gestión de eventos del botón "Traducir"..
+4. Estructurar las pruebas unitarias.
+5. Implementar Casos de pruebas.</t>
+  </si>
+  <si>
+    <t>INCOMPLETO (FALTA IMPLEMENTAR MÁS CARACTERES ESPECIALES)</t>
+  </si>
+  <si>
+    <t>INCOMPLETO (FALTA PASAR TODAS LAS PRUEBAS UNITARIAS)</t>
+  </si>
+  <si>
+    <t>Iteración 1</t>
+  </si>
+  <si>
     <t>Iteración 2</t>
   </si>
   <si>
-    <t>ISWD633 CONTRUCCIÓN Y EVOLUCÍON DEL SOFTWARE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRADUCTOR VERSIÓN: 1.0 </t>
-  </si>
-  <si>
-    <t>FECHA DE PUBLICACIÓN:</t>
-  </si>
-  <si>
-    <t>AUTOR:</t>
-  </si>
-  <si>
-    <t>TEMA:</t>
-  </si>
-  <si>
-    <t>FLUJO DE TRABAJO</t>
-  </si>
-  <si>
-    <t>BrailleTech</t>
+    <t>Iteración 3</t>
   </si>
 </sst>
 </file>
@@ -182,14 +315,13 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -229,7 +361,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -394,40 +526,14 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -443,7 +549,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -453,30 +559,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -494,6 +576,49 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -506,38 +631,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -546,83 +656,104 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -958,296 +1089,548 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36481D96-295F-42A9-B05C-806EDECC9BF8}">
-  <dimension ref="B1:L18"/>
+  <dimension ref="B1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="78" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:K22"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" customWidth="1"/>
     <col min="3" max="6" width="15.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="23.44140625" customWidth="1"/>
     <col min="8" max="8" width="31.5546875" customWidth="1"/>
-    <col min="9" max="9" width="58.88671875" customWidth="1"/>
+    <col min="9" max="9" width="61.21875" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" customWidth="1"/>
     <col min="11" max="11" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="38" t="s">
+    <row r="1" spans="2:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+    </row>
+    <row r="2" spans="2:12" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+    </row>
+    <row r="3" spans="2:12" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="31"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+    </row>
+    <row r="4" spans="2:12" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="31"/>
+      <c r="D4" s="39">
+        <v>45449</v>
+      </c>
+      <c r="E4" s="39"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+    </row>
+    <row r="5" spans="2:12" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="31" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="39" t="s">
+      <c r="C5" s="31"/>
+      <c r="D5" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="38"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+    </row>
+    <row r="6" spans="2:12" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+    </row>
+    <row r="7" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="39"/>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="39" t="s">
+      <c r="C7" s="31"/>
+      <c r="D7" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="40">
-        <v>45449</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="2:12" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="14" t="s">
+      <c r="E7" s="38"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+    </row>
+    <row r="8" spans="2:12" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="17"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="19"/>
+    </row>
+    <row r="9" spans="2:12" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="2:12" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="24"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="2:12" s="17" customFormat="1" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="K10" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" ht="174.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="27" t="s">
-        <v>5</v>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="34"/>
+    </row>
+    <row r="10" spans="2:12" s="9" customFormat="1" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="35"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="37"/>
+    </row>
+    <row r="11" spans="2:12" ht="174.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="14" t="s">
+        <v>21</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D11" s="29"/>
       <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="30" t="s">
+      <c r="F11" s="30"/>
+      <c r="G11" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="L11" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="174.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="L12" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="174.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="41"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="L13" s="25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="174.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="41"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="31" t="s">
+      <c r="H14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" s="25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="144" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="41"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="30" t="s">
+      <c r="I15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="K11" s="32" t="s">
+      <c r="K15" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" s="25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="144" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="L16" s="25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="189.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="41"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K17" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L17" s="25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="214.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="41"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="L18" s="25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" ht="240" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="41"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="L19" s="25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K20" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="L20" s="25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="139.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="41"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21" s="21" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="2:12" ht="174.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="5"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4" t="s">
+      <c r="L21" s="25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="300.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="41"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" ht="174.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="5"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="4" t="s">
+      <c r="H22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="L22" s="25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="330" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="42"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" ht="174.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" ht="144" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="H15" s="22"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="23"/>
-    </row>
-    <row r="16" spans="2:12" ht="144" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="5"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="6"/>
-    </row>
-    <row r="17" spans="2:11" ht="144" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="5"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="6"/>
-    </row>
-    <row r="18" spans="2:11" ht="144" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="10"/>
+      <c r="H23" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K23" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="L23" s="26" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="B8:K9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="B2:C2"/>
+  <mergeCells count="14">
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B1:L2"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="B16:B19"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B9:L10"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>